<commit_message>
Cmbios, se sube la app completa en nuevo folder
</commit_message>
<xml_diff>
--- a/control_de_facturacion_2025.xlsx
+++ b/control_de_facturacion_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,6 +500,756 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>987</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cosas </t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" t="n">
+        <v>550</v>
+      </c>
+      <c r="K2" t="n">
+        <v>88</v>
+      </c>
+      <c r="L2" t="n">
+        <v>638</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>987</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>cosas1</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="n">
+        <v>550</v>
+      </c>
+      <c r="K3" t="n">
+        <v>88</v>
+      </c>
+      <c r="L3" t="n">
+        <v>638</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>987</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>cosas2</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" t="n">
+        <v>550</v>
+      </c>
+      <c r="K4" t="n">
+        <v>88</v>
+      </c>
+      <c r="L4" t="n">
+        <v>638</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>987</v>
+      </c>
+      <c r="E5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>cosas3</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" t="n">
+        <v>550</v>
+      </c>
+      <c r="K5" t="n">
+        <v>88</v>
+      </c>
+      <c r="L5" t="n">
+        <v>638</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>987</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>cosas4</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>550</v>
+      </c>
+      <c r="K6" t="n">
+        <v>88</v>
+      </c>
+      <c r="L6" t="n">
+        <v>638</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>987</v>
+      </c>
+      <c r="E7" t="n">
+        <v>9</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>cosas5</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>6</v>
+      </c>
+      <c r="J7" t="n">
+        <v>550</v>
+      </c>
+      <c r="K7" t="n">
+        <v>88</v>
+      </c>
+      <c r="L7" t="n">
+        <v>638</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>kasdn_2025-03-11_092809.xlsx</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>RFC.  123456789000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>materiales 1</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>15</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="L8" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>kasdn_2025-03-11_092809.xlsx</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>RFC.  123456789000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>materiales 2</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" t="n">
+        <v>15</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="L9" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>987</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cosas </t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>100</v>
+      </c>
+      <c r="J10" t="n">
+        <v>550</v>
+      </c>
+      <c r="K10" t="n">
+        <v>88</v>
+      </c>
+      <c r="L10" t="n">
+        <v>638</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>987</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>cosas1</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" t="n">
+        <v>550</v>
+      </c>
+      <c r="K11" t="n">
+        <v>88</v>
+      </c>
+      <c r="L11" t="n">
+        <v>638</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>987</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>cosas2</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" t="n">
+        <v>550</v>
+      </c>
+      <c r="K12" t="n">
+        <v>88</v>
+      </c>
+      <c r="L12" t="n">
+        <v>638</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>987</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>cosas3</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>4</v>
+      </c>
+      <c r="J13" t="n">
+        <v>550</v>
+      </c>
+      <c r="K13" t="n">
+        <v>88</v>
+      </c>
+      <c r="L13" t="n">
+        <v>638</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>987</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>cosas4</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>5</v>
+      </c>
+      <c r="J14" t="n">
+        <v>550</v>
+      </c>
+      <c r="K14" t="n">
+        <v>88</v>
+      </c>
+      <c r="L14" t="n">
+        <v>638</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2_2025-03-11_112013.xlsx</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Marcas y representaciones SA. de CV.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>987</v>
+      </c>
+      <c r="E15" t="n">
+        <v>9</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>cosas5</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>6</v>
+      </c>
+      <c r="J15" t="n">
+        <v>550</v>
+      </c>
+      <c r="K15" t="n">
+        <v>88</v>
+      </c>
+      <c r="L15" t="n">
+        <v>638</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
subiendo archivo estandar de prueba
</commit_message>
<xml_diff>
--- a/control_de_facturacion_2025.xlsx
+++ b/control_de_facturacion_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,16 @@
           <t>Tipo de moneda</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Responsable de facturación</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Razón social</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -560,6 +570,14 @@
           <t>MXN</t>
         </is>
       </c>
+      <c r="O2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -616,6 +634,14 @@
           <t>MXN</t>
         </is>
       </c>
+      <c r="O3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -672,6 +698,14 @@
           <t>MXN</t>
         </is>
       </c>
+      <c r="O4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -728,6 +762,14 @@
           <t>MXN</t>
         </is>
       </c>
+      <c r="O5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -784,6 +826,14 @@
           <t>MXN</t>
         </is>
       </c>
+      <c r="O6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -840,6 +890,14 @@
           <t>MXN</t>
         </is>
       </c>
+      <c r="O7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -896,6 +954,14 @@
           <t>MXN</t>
         </is>
       </c>
+      <c r="O8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -956,6 +1022,16 @@
           <t>DLLS</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1012,6 +1088,16 @@
         </is>
       </c>
       <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1068,6 +1154,16 @@
         </is>
       </c>
       <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1124,6 +1220,16 @@
         </is>
       </c>
       <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1180,6 +1286,16 @@
         </is>
       </c>
       <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1236,6 +1352,16 @@
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1292,6 +1418,16 @@
         </is>
       </c>
       <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1344,6 +1480,16 @@
         </is>
       </c>
       <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1400,6 +1546,16 @@
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>